<commit_message>
Test für empty text
</commit_message>
<xml_diff>
--- a/Templates/Json_Excel_Template_Scala.xlsx
+++ b/Templates/Json_Excel_Template_Scala.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FloraValentina/Library/Mobile Documents/com~apple~CloudDocs/Dokumente/Arbeit/Onesome/Coding/Jsons/Json Builder/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56D7F73-72D5-514F-AB09-5E785F2DF816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4609A79E-A5DC-1348-9D3D-ABC2BAB5D270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{10C9D494-FF19-E541-B5E6-AA7C08DB1016}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="1" xr2:uid="{10C9D494-FF19-E541-B5E6-AA7C08DB1016}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
   <si>
     <t>Text</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>MORE_INFORMATION</t>
-  </si>
-  <si>
-    <t>audio_file_name.wav</t>
   </si>
   <si>
     <t>Hier kann der Text einfach frei gelassen werden und es werden mehrere Antwortmöglichkeiten eingefügt wie zb. unter einer item list oder eine lila wolke</t>
@@ -383,7 +380,23 @@
     <t>Das ein Beispiel Paragraph für Frage 4</t>
   </si>
   <si>
-    <t>1(wenig motiviert)-5(sehr motiviert)</t>
+    <t>audio_file_name.png</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Benutze das, um eine Scala als Antwortmöglichkeit einzufügen. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Textkörper)"/>
+      </rPr>
+      <t>Achtung: der Text muss immer wie folgt aussehen: minimumZahl(text für minimum)-maximumZahl(text für maximum). Beispiel: 0(wenig motiviert)-5(sehr motiviert)</t>
+    </r>
+  </si>
+  <si>
+    <t>0(wenig motiviert)-5(sehr motiviert)</t>
   </si>
 </sst>
 </file>
@@ -923,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA3210E-E7A6-2043-8156-8087E806CB00}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,10 +964,10 @@
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="12">
         <v>1</v>
@@ -1000,25 +1013,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K2"/>
     </row>
@@ -1033,25 +1046,25 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -1066,25 +1079,25 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -1098,13 +1111,13 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5"/>
@@ -1120,13 +1133,13 @@
         <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6"/>
@@ -1142,7 +1155,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -1157,18 +1170,18 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="272" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="34" x14ac:dyDescent="0.2">
@@ -1176,25 +1189,25 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -1219,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2357A5-20B8-E04D-B005-78DA48C95BE8}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1235,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1243,7 +1256,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -1251,7 +1264,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -1259,7 +1272,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="85" x14ac:dyDescent="0.2">
@@ -1267,15 +1280,15 @@
         <v>21</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="68" x14ac:dyDescent="0.2">
@@ -1283,7 +1296,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="68" x14ac:dyDescent="0.2">
@@ -1291,29 +1304,31 @@
         <v>5</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="14"/>
+        <v>56</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="119" x14ac:dyDescent="0.2">
@@ -1321,7 +1336,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>